<commit_message>
Add order number field to orders table
</commit_message>
<xml_diff>
--- a/client/src/assets/sample/ctordering_orders.xlsx
+++ b/client/src/assets/sample/ctordering_orders.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Softices/personal/workspace/ruby/foodup-github/client/src/assets/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ORDER_ID</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>VALUE</t>
+  </si>
+  <si>
+    <t>ORDER_NUMBER</t>
   </si>
 </sst>
 </file>
@@ -430,66 +433,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 D1:E1 B1 F1 G1:K1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 E1:F1 C1 G1 H1:L1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>